<commit_message>
Add Gender Column and Update Filters, Views ,Requests
</commit_message>
<xml_diff>
--- a/public/assets_v1/import_example/Users Example.xlsx
+++ b/public/assets_v1/import_example/Users Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programs\laragon\www\arabicArabs\public\assets_v1\import_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B533B762-AC68-4643-8A94-5E57550BB126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BB3A80-F773-4C9F-B445-3D7FB4447CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Email</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>1 to 13</t>
+  </si>
+  <si>
+    <t>Gender</t>
   </si>
 </sst>
 </file>
@@ -458,7 +461,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,9 +599,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P17" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>